<commit_message>
Fix submit and Update README
</commit_message>
<xml_diff>
--- a/API README.xlsx
+++ b/API README.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kisumi\Documents\bootcamp\fs8-MVP-1-Naaomo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B165C1D-D0E1-4714-B635-AE98EB09892A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87386A12-2BAA-4815-8C4C-220AAD9CA188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C040E827-9410-44A1-B502-823AFC3854A5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>URL</t>
   </si>
@@ -104,6 +104,30 @@
   </si>
   <si>
     <t>{text: STRING}</t>
+  </si>
+  <si>
+    <t>/pets/pettype</t>
+  </si>
+  <si>
+    <t>Get all the pet types</t>
+  </si>
+  <si>
+    <t>id: AUTO ID
+pet_type: Cat, Dog, Hedgehog, Oceanic, Reptiles, Exotics, Others</t>
+  </si>
+  <si>
+    <t>/pets/createpet</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Create a new pet</t>
+  </si>
+  <si>
+    <t>petname: STRING,
+petimg: STRING,
+pettype_id: AUTO</t>
   </si>
 </sst>
 </file>
@@ -214,11 +238,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -230,6 +251,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -548,96 +575,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E085F0D-4F3F-427A-8F5F-82867B1BAFFB}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="144.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -646,7 +701,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{D6179EE0-8FCF-4811-8BD2-DEE9C793E3F7}"/>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{D6179EE0-8FCF-4811-8BD2-DEE9C793E3F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>